<commit_message>
Commit of the updated file via cmd Windows
</commit_message>
<xml_diff>
--- a/certificates_list.xlsx
+++ b/certificates_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Link to cert</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Chrome DevTools</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -473,6 +476,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.1796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -535,13 +539,20 @@
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1">
         <v>2022</v>
       </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -551,6 +562,7 @@
     <hyperlink ref="B3" r:id="rId4"/>
     <hyperlink ref="A4" r:id="rId5"/>
     <hyperlink ref="A5" r:id="rId6"/>
+    <hyperlink ref="A7" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>